<commit_message>
my new running extent
</commit_message>
<xml_diff>
--- a/haltungcrm/src/test/resources/data/Book1.xlsx
+++ b/haltungcrm/src/test/resources/data/Book1.xlsx
@@ -4,25 +4,31 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17220" windowHeight="5208"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17220" windowHeight="8004" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="edit" sheetId="1" r:id="rId1"/>
+    <sheet name="delete" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O16"/>
+  <oleSize ref="A1:Q26"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>reddy</t>
   </si>
   <si>
     <t>campaign name</t>
+  </si>
+  <si>
+    <t>lakshma</t>
+  </si>
+  <si>
+    <t>Infosys</t>
   </si>
 </sst>
 </file>
@@ -366,8 +372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -386,7 +392,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3"/>
@@ -398,12 +408,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>